<commit_message>
spreadsheet: add complex example
This has some conditional formatting, charts and auto filters.
</commit_message>
<xml_diff>
--- a/_examples/spreadsheet/complex/complex.xlsx
+++ b/_examples/spreadsheet/complex/complex.xlsx
@@ -44,18 +44,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
-  <x:fonts count="1">
+  <x:fonts count="2">
     <x:font>
       <x:name val="Calibri"/>
       <x:sz val="11"/>
     </x:font>
+    <x:font>
+      <x:b/>
+    </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="3">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="ffd3d3d3"/>
+      </x:patternFill>
     </x:fill>
   </x:fills>
   <x:borders count="1">
@@ -70,8 +78,9 @@
   <x:cellStyleXfs count="1">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf fontId="1" fillId="2" applyFont="1" applyFill="1"/>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,13 +480,13 @@
 <xdr:wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -498,15 +507,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -529,18 +538,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
   <x:dimension ref="A1"/>
+  <x:cols>
+    <x:col min="1" max="1" width="15.428571428571429"/>
+    <x:col min="4" max="4" width="20.571428571428573"/>
+  </x:cols>
   <x:sheetData>
     <x:row r="1">
-      <x:c r="A1" t="s">
+      <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" t="s">
+      <x:c r="B1" s="1" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" t="s">
+      <x:c r="C1" s="1" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" t="s">
+      <x:c r="D1" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
document/spreadsheet: updates for new schema
</commit_message>
<xml_diff>
--- a/_examples/spreadsheet/complex/complex.xlsx
+++ b/_examples/spreadsheet/complex/complex.xlsx
@@ -1,95 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
-  <x:sheets>
-    <x:sheet name="Sheet 1" sheetId="1" r:id="rId3"/>
-  </x:sheets>
-  <x:definedNames>
-    <x:definedName name="_xlnm._FilterDatabase" localSheetId="0">'Sheet 1'!$A$1:$D$6</x:definedName>
-  </x:definedNames>
-</x:workbook>
+<ma:workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+  <ma:sheets>
+    <ma:sheet name="Sheet 1" sheetId="1" r:id="rId3"/>
+  </ma:sheets>
+  <ma:definedNames>
+    <ma:definedName name="_xlnm._FilterDatabase" localSheetId="0">'Sheet 1'!$A$1:$D$6</ma:definedName>
+  </ma:definedNames>
+</ma:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" count="9" uniqueCount="9">
-  <x:si>
-    <x:t>Item</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Price</x:t>
-  </x:si>
-  <x:si>
-    <x:t># Sold</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Total</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product 4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Product 5</x:t>
-  </x:si>
-</x:sst>
+<ma:sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" count="9" uniqueCount="9">
+  <ma:si>
+    <ma:t>Item</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Price</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t># Sold</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Total</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Product 1</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Product 2</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Product 3</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Product 4</ma:t>
+  </ma:si>
+  <ma:si>
+    <ma:t>Product 5</ma:t>
+  </ma:si>
+</ma:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<x:styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
-  <x:fonts count="2">
-    <x:font>
-      <x:name val="Calibri"/>
-      <x:sz val="11"/>
-    </x:font>
-    <x:font>
-      <x:b/>
-    </x:font>
-  </x:fonts>
-  <x:fills count="3">
-    <x:fill>
-      <x:patternFill patternType="none"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="gray125"/>
-    </x:fill>
-    <x:fill>
-      <x:patternFill patternType="solid">
-        <x:fgColor rgb="ffd3d3d3"/>
-      </x:patternFill>
-    </x:fill>
-  </x:fills>
-  <x:borders count="1">
-    <x:border>
-      <x:left/>
-      <x:right/>
-      <x:top/>
-      <x:bottom/>
-      <x:diagonal/>
-    </x:border>
-  </x:borders>
-  <x:cellStyleXfs count="1">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </x:cellStyleXfs>
-  <x:cellXfs count="2">
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf fontId="1" fillId="2" applyFont="1" applyFill="1"/>
-  </x:cellXfs>
-  <x:cellStyles count="1">
-    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </x:cellStyles>
-</x:styleSheet>
+<ma:styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+  <ma:fonts count="2">
+    <ma:font>
+      <ma:name val="Calibri"/>
+      <ma:sz val="11"/>
+    </ma:font>
+    <ma:font>
+      <ma:b/>
+    </ma:font>
+  </ma:fonts>
+  <ma:fills count="3">
+    <ma:fill>
+      <ma:patternFill patternType="none"/>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="gray125"/>
+    </ma:fill>
+    <ma:fill>
+      <ma:patternFill patternType="solid">
+        <ma:fgColor rgb="ffd3d3d3"/>
+      </ma:patternFill>
+    </ma:fill>
+  </ma:fills>
+  <ma:borders count="1">
+    <ma:border>
+      <ma:left/>
+      <ma:right/>
+      <ma:top/>
+      <ma:bottom/>
+      <ma:diagonal/>
+    </ma:border>
+  </ma:borders>
+  <ma:cellStyleXfs count="1">
+    <ma:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </ma:cellStyleXfs>
+  <ma:cellXfs count="2">
+    <ma:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <ma:xf fontId="1" fillId="2" applyFont="1" applyFill="1"/>
+  </ma:cellXfs>
+  <ma:cellStyles count="1">
+    <ma:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </ma:cellStyles>
+</ma:styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+<c:chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace">
   <c:chart>
     <c:title>
       <c:tx>
@@ -258,7 +258,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+<c:chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace">
   <c:chart>
     <c:title>
       <c:tx>
@@ -499,7 +499,7 @@
       <xdr:xfrm/>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace" r:id="rId1"/>
+          <c:chart xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -526,7 +526,7 @@
       <xdr:xfrm/>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace" r:id="rId2"/>
+          <c:chart xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xml="http://www.w3.org/XML/1998/namespace" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -536,120 +536,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
-  <x:dimension ref="A1"/>
-  <x:cols>
-    <x:col min="1" max="1" width="15.428571428571429"/>
-    <x:col min="4" max="4" width="20.571428571428573"/>
-  </x:cols>
-  <x:sheetData>
-    <x:row r="1">
-      <x:c r="A1" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B1" s="1" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="1" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="D1" s="1" t="s">
-        <x:v>3</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2">
-      <x:c r="A2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="B2" t="n">
-        <x:v>3.1</x:v>
-      </x:c>
-      <x:c r="C2" t="n">
-        <x:v>38</x:v>
-      </x:c>
-      <x:c r="D2" t="str">
-        <x:f>C2*B2</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="3">
-      <x:c r="A3" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B3" t="n">
-        <x:v>4.7</x:v>
-      </x:c>
-      <x:c r="C3" t="n">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="D3" t="str">
-        <x:f>C3*B3</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="4">
-      <x:c r="A4" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B4" t="n">
-        <x:v>3.1</x:v>
-      </x:c>
-      <x:c r="C4" t="n">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="D4" t="str">
-        <x:f>C4*B4</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="5">
-      <x:c r="A5" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B5" t="n">
-        <x:v>2.5</x:v>
-      </x:c>
-      <x:c r="C5" t="n">
-        <x:v>41</x:v>
-      </x:c>
-      <x:c r="D5" t="str">
-        <x:f>C5*B5</x:f>
-      </x:c>
-    </x:row>
-    <x:row r="6">
-      <x:c r="A6" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B6" t="n">
-        <x:v>0.6</x:v>
-      </x:c>
-      <x:c r="C6" t="n">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="D6" t="str">
-        <x:f>C6*B6</x:f>
-      </x:c>
-    </x:row>
-  </x:sheetData>
-  <x:autoFilter ref="A1:D6"/>
-  <x:conditionalFormatting sqref="D2:D6">
-    <x:cfRule type="dataBar" priority="2">
-      <x:dataBar minLength="10" maxLength="90" showValue="1">
-        <x:cfvo type="min" val="0"/>
-        <x:cfvo type="max" val="0"/>
-        <x:color rgb="ff0000ff"/>
-      </x:dataBar>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:conditionalFormatting sqref="B2:B6">
-    <x:cfRule type="colorScale" priority="2">
-      <x:colorScale>
-        <x:cfvo type="min" val="0"/>
-        <x:cfvo type="percentile" val="50"/>
-        <x:cfvo type="max" val="0"/>
-        <x:color rgb="ff00cc00"/>
-        <x:color rgb="ffffa500"/>
-        <x:color rgb="ffff0000"/>
-      </x:colorScale>
-    </x:cfRule>
-  </x:conditionalFormatting>
-  <x:drawing r:id="rId1"/>
-</x:worksheet>
+<ma:worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ma="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace">
+  <ma:dimension ref="A1"/>
+  <ma:cols>
+    <ma:col min="1" max="1" width="15.428571428571429"/>
+    <ma:col min="4" max="4" width="20.571428571428573"/>
+  </ma:cols>
+  <ma:sheetData>
+    <ma:row r="1">
+      <ma:c r="A1" s="1" t="s">
+        <ma:v>0</ma:v>
+      </ma:c>
+      <ma:c r="B1" s="1" t="s">
+        <ma:v>1</ma:v>
+      </ma:c>
+      <ma:c r="C1" s="1" t="s">
+        <ma:v>2</ma:v>
+      </ma:c>
+      <ma:c r="D1" s="1" t="s">
+        <ma:v>3</ma:v>
+      </ma:c>
+    </ma:row>
+    <ma:row r="2">
+      <ma:c r="A2" t="s">
+        <ma:v>4</ma:v>
+      </ma:c>
+      <ma:c r="B2" t="n">
+        <ma:v>3.1</ma:v>
+      </ma:c>
+      <ma:c r="C2" t="n">
+        <ma:v>38</ma:v>
+      </ma:c>
+      <ma:c r="D2" t="str">
+        <ma:f>C2*B2</ma:f>
+      </ma:c>
+    </ma:row>
+    <ma:row r="3">
+      <ma:c r="A3" t="s">
+        <ma:v>5</ma:v>
+      </ma:c>
+      <ma:c r="B3" t="n">
+        <ma:v>4.7</ma:v>
+      </ma:c>
+      <ma:c r="C3" t="n">
+        <ma:v>10</ma:v>
+      </ma:c>
+      <ma:c r="D3" t="str">
+        <ma:f>C3*B3</ma:f>
+      </ma:c>
+    </ma:row>
+    <ma:row r="4">
+      <ma:c r="A4" t="s">
+        <ma:v>6</ma:v>
+      </ma:c>
+      <ma:c r="B4" t="n">
+        <ma:v>3.1</ma:v>
+      </ma:c>
+      <ma:c r="C4" t="n">
+        <ma:v>19</ma:v>
+      </ma:c>
+      <ma:c r="D4" t="str">
+        <ma:f>C4*B4</ma:f>
+      </ma:c>
+    </ma:row>
+    <ma:row r="5">
+      <ma:c r="A5" t="s">
+        <ma:v>7</ma:v>
+      </ma:c>
+      <ma:c r="B5" t="n">
+        <ma:v>2.5</ma:v>
+      </ma:c>
+      <ma:c r="C5" t="n">
+        <ma:v>41</ma:v>
+      </ma:c>
+      <ma:c r="D5" t="str">
+        <ma:f>C5*B5</ma:f>
+      </ma:c>
+    </ma:row>
+    <ma:row r="6">
+      <ma:c r="A6" t="s">
+        <ma:v>8</ma:v>
+      </ma:c>
+      <ma:c r="B6" t="n">
+        <ma:v>0.6</ma:v>
+      </ma:c>
+      <ma:c r="C6" t="n">
+        <ma:v>1</ma:v>
+      </ma:c>
+      <ma:c r="D6" t="str">
+        <ma:f>C6*B6</ma:f>
+      </ma:c>
+    </ma:row>
+  </ma:sheetData>
+  <ma:autoFilter ref="A1:D6"/>
+  <ma:conditionalFormatting sqref="D2:D6">
+    <ma:cfRule type="dataBar" priority="2">
+      <ma:dataBar minLength="10" maxLength="90" showValue="1">
+        <ma:cfvo type="min" val="0"/>
+        <ma:cfvo type="max" val="0"/>
+        <ma:color rgb="ff0000ff"/>
+      </ma:dataBar>
+    </ma:cfRule>
+  </ma:conditionalFormatting>
+  <ma:conditionalFormatting sqref="B2:B6">
+    <ma:cfRule type="colorScale" priority="2">
+      <ma:colorScale>
+        <ma:cfvo type="min" val="0"/>
+        <ma:cfvo type="percentile" val="50"/>
+        <ma:cfvo type="max" val="0"/>
+        <ma:color rgb="ff00cc00"/>
+        <ma:color rgb="ffffa500"/>
+        <ma:color rgb="ffff0000"/>
+      </ma:colorScale>
+    </ma:cfRule>
+  </ma:conditionalFormatting>
+  <ma:drawing r:id="rId1"/>
+</ma:worksheet>
 </file>
</xml_diff>